<commit_message>
update with new logo and colors
</commit_message>
<xml_diff>
--- a/ValueSet-auto-differential-blood-vs.xlsx
+++ b/ValueSet-auto-differential-blood-vs.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
   <si>
     <t>Property</t>
   </si>
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.6</t>
+    <t>0.1.7</t>
   </si>
   <si>
     <t>Name</t>
@@ -48,7 +48,7 @@
     <t>Status</t>
   </si>
   <si>
-    <t>active</t>
+    <t>draft</t>
   </si>
   <si>
     <t>Experimental</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-05-05T10:50:04-05:00</t>
+    <t>2024-08-23T10:17:11-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -72,7 +72,16 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>No display for ContactDetail</t>
+    <t>The Medical College of Wisconsin, Inc. and the National Marrow Donor Program (http://www.cibmtr.org)</t>
+  </si>
+  <si>
+    <t>Bob Milius (bmilius@nmdp.org)</t>
+  </si>
+  <si>
+    <t>Jurisdiction</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>Description</t>
@@ -199,9 +208,6 @@
   </si>
   <si>
     <t>Other cells [#/volume] in Blood by Automated count</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>System URI</t>
@@ -329,10 +335,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true" applyFont="true">
       <alignment vertical="top" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -341,7 +347,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -436,35 +442,43 @@
         <v>18</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="B13" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="B13" t="s" s="2">
+        <v>9</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>23</v>
-      </c>
-      <c r="B15" t="s" s="2">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s" s="2">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -486,170 +500,170 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>62</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>